<commit_message>
update paper table data
</commit_message>
<xml_diff>
--- a/src/papers/paper_table.xlsx
+++ b/src/papers/paper_table.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avaj0001/Documents/reports/papers/phd_thesis/src/papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D26AAFC-E746-454A-93DD-78EBB7A3E6BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{72EAEAEA-E564-F74E-BFC5-AEBB6D18A752}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{158CB650-17ED-EB43-B245-3223EDF23397}"/>
+    <workbookView xWindow="640" yWindow="0" windowWidth="28160" windowHeight="18000" activeTab="1" xr2:uid="{158CB650-17ED-EB43-B245-3223EDF23397}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="paper_table" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">paper_table!$A$2:$E$6</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
   <si>
     <t>Thesis Chapter</t>
   </si>
@@ -415,6 +419,9 @@
     </r>
   </si>
   <si>
+    <t>Co-authors and Contributions</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <i/>
@@ -434,18 +441,167 @@
       </rPr>
       <t xml:space="preserve">
 - Software development
-- Testing aand analysis</t>
-    </r>
-  </si>
-  <si>
-    <t>Co-authors and Contributions</t>
+- Testing and analysis</t>
+    </r>
+  </si>
+  <si>
+    <t>Publication</t>
+  </si>
+  <si>
+    <t>Student Contribution</t>
+  </si>
+  <si>
+    <t>Co-authors Contributions</t>
+  </si>
+  <si>
+    <t>A follow-up on</t>
+  </si>
+  <si>
+    <t>Rory Smith (7%)</t>
+  </si>
+  <si>
+    <t>intermediate-mass</t>
+  </si>
+  <si>
+    <t>- Concept development</t>
+  </si>
+  <si>
+    <t>black hole candidates</t>
+  </si>
+  <si>
+    <t>- Data analysis</t>
+  </si>
+  <si>
+    <t>- Interpretation</t>
+  </si>
+  <si>
+    <t>in the second LVK</t>
+  </si>
+  <si>
+    <t>- Paper writing</t>
+  </si>
+  <si>
+    <t>- Editorial assistance</t>
+  </si>
+  <si>
+    <t>observing run with the</t>
+  </si>
+  <si>
+    <t>Eric Thrane (7%)</t>
+  </si>
+  <si>
+    <t>Bayes Coherence Ratio</t>
+  </si>
+  <si>
+    <t>Gregory Ashton (4%)</t>
+  </si>
+  <si>
+    <t>- Software development</t>
+  </si>
+  <si>
+    <t>Other authors (2%)</t>
+  </si>
+  <si>
+    <t>- Editorial assistance.</t>
+  </si>
+  <si>
+    <t>Measuring the</t>
+  </si>
+  <si>
+    <t>Other authors (20%)</t>
+  </si>
+  <si>
+    <t>properties of</t>
+  </si>
+  <si>
+    <t>active galactic nuclei</t>
+  </si>
+  <si>
+    <t>disks with</t>
+  </si>
+  <si>
+    <t>gravitational waves</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Theoretical Expertise</t>
+    </r>
+  </si>
+  <si>
+    <t>Deep follow-up of</t>
+  </si>
+  <si>
+    <t>Returned</t>
+  </si>
+  <si>
+    <t>Rory Smith (10%)</t>
+  </si>
+  <si>
+    <t>GW151226:</t>
+  </si>
+  <si>
+    <t>for</t>
+  </si>
+  <si>
+    <t>ordinary binary or</t>
+  </si>
+  <si>
+    <t>revison</t>
+  </si>
+  <si>
+    <t>low-mass-ratio</t>
+  </si>
+  <si>
+    <t>system?</t>
+  </si>
+  <si>
+    <t>Eric Thrane (10%)</t>
+  </si>
+  <si>
+    <t>Dan Foreman-Mackey (20%)</t>
+  </si>
+  <si>
+    <t>Massively parallel</t>
+  </si>
+  <si>
+    <t>Rory Smith (40%)</t>
+  </si>
+  <si>
+    <t>Bayesian inference</t>
+  </si>
+  <si>
+    <t>for transient</t>
+  </si>
+  <si>
+    <t>- Testing and analysis</t>
+  </si>
+  <si>
+    <t>gravitational-wave</t>
+  </si>
+  <si>
+    <t>astronomy</t>
+  </si>
+  <si>
+    <t>Gregory Ashton (35%)</t>
+  </si>
+  <si>
+    <t>Colm Talbot (5%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -493,13 +649,37 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -514,7 +694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -537,6 +717,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,37 +748,7 @@
   <dxfs count="13">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -665,7 +839,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -722,7 +896,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -764,7 +938,37 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -795,7 +999,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E4B778B-08DF-3045-9036-02CEBFC1F216}" name="Table1" displayName="Table1" ref="A1:E6" headerRowDxfId="2" dataDxfId="0" totalsRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E4B778B-08DF-3045-9036-02CEBFC1F216}" name="Table1" displayName="Table1" ref="A1:E6" headerRowDxfId="12" dataDxfId="11" totalsRowDxfId="10">
   <autoFilter ref="A1:E6" xr:uid="{87E2C400-5080-E245-82D3-7F957E8551C9}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -804,11 +1008,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B5378837-4AC8-6A4F-AC20-68674BECD4EA}" name="Thesis Chapter" totalsRowLabel="Total" dataDxfId="7" totalsRowDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{22CB1FA9-EBEB-B44B-B404-28832A3D74AF}" name="Publication Title" dataDxfId="6" totalsRowDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{8DE42504-4910-FB41-A18E-25C988845D7F}" name="Status" dataDxfId="5" totalsRowDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{C49431F8-6683-4540-93B7-F92AB579C29A}" name="Nature and % of Student Contribution" dataDxfId="4" totalsRowDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{5DA21EA2-D563-8346-8D09-282D846A9105}" name="Co-authors and Contributions" totalsRowFunction="count" dataDxfId="3" totalsRowDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{B5378837-4AC8-6A4F-AC20-68674BECD4EA}" name="Thesis Chapter" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{22CB1FA9-EBEB-B44B-B404-28832A3D74AF}" name="Publication Title" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{8DE42504-4910-FB41-A18E-25C988845D7F}" name="Status" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{C49431F8-6683-4540-93B7-F92AB579C29A}" name="Nature and % of Student Contribution" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{5DA21EA2-D563-8346-8D09-282D846A9105}" name="Co-authors and Contributions" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1111,19 +1315,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65DF7A6B-C2E0-1149-9DF1-4284C1AF2A95}">
-  <dimension ref="A1:F9"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="E6" sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="4" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="39.33203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="39" style="4" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="38.5" style="4" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
@@ -1141,7 +1348,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="209">
@@ -1223,7 +1430,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>19</v>
@@ -1241,9 +1448,507 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="73" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC9C1859-F94D-5746-8EDE-A9BB62343319}">
+  <dimension ref="A1:F40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="2.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18">
+      <c r="A1" s="8"/>
+      <c r="B1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" ht="18">
+      <c r="A2" s="11">
+        <v>2</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18">
+      <c r="A4" s="14"/>
+      <c r="B4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18">
+      <c r="A5" s="14"/>
+      <c r="B5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18">
+      <c r="A6" s="14"/>
+      <c r="B6" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18">
+      <c r="A7" s="14"/>
+      <c r="B7" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="18">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="18">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="18">
+      <c r="A14" s="11">
+        <v>5</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="18">
+      <c r="A15" s="14"/>
+      <c r="B15" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="18">
+      <c r="A16" s="14"/>
+      <c r="B16" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18">
+      <c r="A17" s="14"/>
+      <c r="B17" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18">
+      <c r="A18" s="14"/>
+      <c r="B18" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18">
+      <c r="A19" s="11">
+        <v>4</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18">
+      <c r="A20" s="14"/>
+      <c r="B20" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18">
+      <c r="A21" s="14"/>
+      <c r="B21" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18">
+      <c r="A22" s="14"/>
+      <c r="B22" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18">
+      <c r="A23" s="14"/>
+      <c r="B23" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="18">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="18">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="18">
+      <c r="A27" s="11">
+        <v>6</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="18">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="18">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="18">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="18">
+      <c r="A31" s="11">
+        <v>3</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="18">
+      <c r="A32" s="14"/>
+      <c r="B32" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="18">
+      <c r="A33" s="14"/>
+      <c r="B33" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="18">
+      <c r="A34" s="14"/>
+      <c r="B34" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="18">
+      <c r="A35" s="14"/>
+      <c r="B35" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="18">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="18">
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="18">
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="18">
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="18">
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>